<commit_message>
Now the Excel looks better
</commit_message>
<xml_diff>
--- a/maintenance_schedule.xlsx
+++ b/maintenance_schedule.xlsx
@@ -429,12 +429,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Maintenance Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Tasks</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Hours required</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Now the maintenance time is rounded up to .1 hour
</commit_message>
<xml_diff>
--- a/maintenance_schedule.xlsx
+++ b/maintenance_schedule.xlsx
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -549,7 +549,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -699,7 +699,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[4.299999999999999]</t>
+          <t>[4.3]</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -729,7 +729,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[0.30000000000000004]</t>
+          <t>[0.3]</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -759,7 +759,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -834,7 +834,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -894,7 +894,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -984,7 +984,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[4.299999999999999]</t>
+          <t>[4.3]</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[0.30000000000000004]</t>
+          <t>[0.3]</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[4.599999999999998]</t>
+          <t>[4.6]</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[4.299999999999999]</t>
+          <t>[4.3]</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1314,7 +1314,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[4.3999999999999995]</t>
+          <t>[4.4]</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1524,7 +1524,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[4.299999999999999]</t>
+          <t>[4.3]</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1719,7 +1719,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[4.199999999999999]</t>
+          <t>[4.2]</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -1794,7 +1794,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>[4.6999999999999975]</t>
+          <t>[4.7]</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">

</xml_diff>

<commit_message>
Same as with last talk
</commit_message>
<xml_diff>
--- a/maintenance_schedule.xlsx
+++ b/maintenance_schedule.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C94"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,16 +470,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
@@ -489,12 +489,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
@@ -504,27 +504,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>524504-50-01, 353103-00-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
@@ -549,42 +549,42 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
@@ -594,42 +594,42 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>524504-50-01, 353103-00-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>270</v>
+        <v>296</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
@@ -639,33 +639,33 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[0.5]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-01-09, 321100-01-09, 323200-50-01, 323200-50-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -680,76 +680,76 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[6]</t>
+          <t>[4.6]</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>324200-00-05</t>
+          <t>212700-00-01, 262400-00-02, 335000-02-04, 342200-00-01, 341100-50-01, 300000-50-01, 300000-50-01, 300000-50-01</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[4.3]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02, 353103-00-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[4.0]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>212700-00-01, 262400-00-02, 335000-02-04, 342200-00-01, 341100-50-01, 300000-50-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>390</v>
+        <v>420</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[0.3]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>420</v>
+        <v>444</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
@@ -759,168 +759,168 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>455</v>
+        <v>480</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>480</v>
+        <v>510</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>524504-50-01, 353103-00-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>520</v>
+        <v>540</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>540</v>
+        <v>570</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>570</v>
+        <v>592</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>585</v>
+        <v>600</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[0.6]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>524504-50-01, 353103-00-01, 321100-01-09, 321100-01-09, 323200-50-01, 323200-50-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>630</v>
+        <v>660</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>650</v>
+        <v>666</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>660</v>
+        <v>690</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -935,7 +935,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>690</v>
+        <v>720</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -950,67 +950,67 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>700</v>
+        <v>730</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[6]</t>
+          <t>[4.6]</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>324200-00-05</t>
+          <t>212700-00-01, 262400-00-02, 335000-02-04, 342200-00-01, 341100-50-01, 300000-50-01, 300000-50-01, 300000-50-01</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>715</v>
+        <v>740</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[65.1]</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01, 062101-00-01, 062101-00-02, 062103-00-01, 062108-00-01, 062108-20-02, 062202-20-01, 062203-20-01, 062204-00-01, 062302-00-01, 062303-00-01, 062401-00-01, 062401-00-01, 202103-00-01, 202107-00-03, 202108-00-01, 202108-00-02, 202108-00-03, 202108-00-04, 202202-00-01, 202202-00-02, 202203-00-01, 202204-00-01, 202505-00-01, 202605-00-01, 202901-00-02, 213000-00-03, 213000-00-06, 221100-00-03, 222100-00-02, 222100-00-04, 223100-00-01, 223100-00-02, 233100-00-02, 255700-00-04, 255700-00-05, 255700-00-06, 261301-00-02, 261303-00-02, 261303-00-04, 262500-00-05, 270001-00-03, 270001-00-06, 271100-00-06, 273500-03-05, 274200-00-04, 274200-01-12, 276400-00-01, 282200-00-01, 284300-00-01, 290100-00-02, 291300-00-02, 303100-01-01, 303100-01-02, 323100-00-02, 323300-00-03, 324400-00-02, 324400-00-05, 324500-00-01, 341100-00-04, 341200-00-01, 360000-00-02, 360000-00-02, 360000-00-04, 381200-00-02, 521203-00-02, 523002-00-04, 523300-00-08, 524102-00-01, 524104-00-02, 524502-00-01, 524504-00-02, 730000-00-05, 761100-00-04, 761100-00-09, 761300-00-02, 761300-00-06, 783500-02-01</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>720</v>
+        <v>750</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[4.3]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02, 353103-00-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>730</v>
+        <v>780</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[4.0]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>212700-00-01, 262400-00-02, 335000-02-04, 342200-00-01, 341100-50-01, 300000-50-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>750</v>
+        <v>810</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1025,67 +1025,67 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>780</v>
+        <v>814</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[0.3]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-03-09, 321100-03-09</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>810</v>
+        <v>840</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>840</v>
+        <v>870</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>524504-50-01, 353103-00-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>845</v>
+        <v>888</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>870</v>
+        <v>900</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1100,187 +1100,187 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>900</v>
+        <v>930</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[4.6]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02, 321100-01-09, 321100-01-09, 323200-50-01, 323200-50-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>910</v>
+        <v>960</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>930</v>
+        <v>962</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>960</v>
+        <v>990</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>524504-50-01, 353103-00-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>975</v>
+        <v>1000</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[3.9]</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>521102-00-09, 801000-00-02, 801000-00-02, 531019-00-05</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>990</v>
+        <v>1020</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1020</v>
+        <v>1036</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1040</v>
+        <v>1050</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1050</v>
+        <v>1080</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[6.1]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>524504-50-01, 324200-00-05</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1080</v>
+        <v>1095</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[4.3]</t>
+          <t>[4.6]</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02, 353103-00-01</t>
+          <t>212700-00-01, 262400-00-02, 335000-02-04, 342200-00-01, 341100-50-01, 300000-50-01, 300000-50-01, 300000-50-01</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1095</v>
+        <v>1110</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[4.0]</t>
+          <t>[12.1]</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>212700-00-01, 262400-00-02, 335000-02-04, 342200-00-01, 341100-50-01, 300000-50-01</t>
+          <t>524504-50-01, 062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1105</v>
+        <v>1140</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1110</v>
+        <v>1170</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -1295,97 +1295,97 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1140</v>
+        <v>1184</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1170</v>
+        <v>1200</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[4.4]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-03-09, 321100-03-09, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1200</v>
+        <v>1230</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[0.6]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>524504-50-01, 353103-00-01, 321100-01-09, 321100-01-09, 323200-50-01, 323200-50-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1230</v>
+        <v>1258</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1235</v>
+        <v>1260</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1260</v>
+        <v>1290</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>1290</v>
+        <v>1320</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -1400,67 +1400,67 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1300</v>
+        <v>1332</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1320</v>
+        <v>1350</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>524504-50-01, 353103-00-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1350</v>
+        <v>1380</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1365</v>
+        <v>1406</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1380</v>
+        <v>1410</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -1475,82 +1475,82 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1400</v>
+        <v>1440</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[6]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>324200-00-05</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1410</v>
+        <v>1460</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[4.6]</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>212700-00-01, 262400-00-02, 335000-02-04, 342200-00-01, 341100-50-01, 300000-50-01, 300000-50-01, 300000-50-01</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>1430</v>
+        <v>1470</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1440</v>
+        <v>1480</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[4.3]</t>
+          <t>[65.1]</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02, 353103-00-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01, 062101-00-01, 062101-00-02, 062103-00-01, 062108-00-01, 062108-20-02, 062202-20-01, 062203-20-01, 062204-00-01, 062302-00-01, 062303-00-01, 062401-00-01, 062401-00-01, 202103-00-01, 202107-00-03, 202108-00-01, 202108-00-02, 202108-00-03, 202108-00-04, 202202-00-01, 202202-00-02, 202203-00-01, 202204-00-01, 202505-00-01, 202605-00-01, 202901-00-02, 213000-00-03, 213000-00-06, 221100-00-03, 222100-00-02, 222100-00-04, 223100-00-01, 223100-00-02, 233100-00-02, 255700-00-04, 255700-00-05, 255700-00-06, 261301-00-02, 261303-00-02, 261303-00-04, 262500-00-05, 270001-00-03, 270001-00-06, 271100-00-06, 273500-03-05, 274200-00-04, 274200-01-12, 276400-00-01, 282200-00-01, 284300-00-01, 290100-00-02, 291300-00-02, 303100-01-01, 303100-01-02, 323100-00-02, 323300-00-03, 324400-00-02, 324400-00-05, 324500-00-01, 341100-00-04, 341200-00-01, 360000-00-02, 360000-00-02, 360000-00-04, 381200-00-02, 521203-00-02, 523002-00-04, 523300-00-08, 524102-00-01, 524104-00-02, 524502-00-01, 524504-00-02, 730000-00-05, 761100-00-04, 761100-00-09, 761300-00-02, 761300-00-06, 783500-02-01</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1460</v>
+        <v>1500</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[4.0]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>212700-00-01, 262400-00-02, 335000-02-04, 342200-00-01, 341100-50-01, 300000-50-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1470</v>
+        <v>1530</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -1565,271 +1565,211 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>1495</v>
+        <v>1554</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1500</v>
+        <v>1560</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[0.5]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-01-09, 321100-01-09, 323200-50-01, 323200-50-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>1530</v>
+        <v>1590</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>1560</v>
+        <v>1620</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[0.4]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-03-09, 321100-03-09, 353103-00-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>1590</v>
+        <v>1628</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>1620</v>
+        <v>1650</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1625</v>
+        <v>1680</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>1650</v>
+        <v>1702</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1680</v>
+        <v>1710</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>524504-50-01, 353103-00-01</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1690</v>
+        <v>1740</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>1710</v>
+        <v>1770</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[4.2]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>1740</v>
+        <v>1776</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>[0.1]</t>
+          <t>[12.0]</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>524504-50-01</t>
+          <t>062403-00-01, 062403-00-01, 215000-00-09, 241000-00-02, 241000-00-02, 254201-00-01, 255100-00-01, 273500-00-01, 491000-00-02, 725200-00-02, 725200-00-02, 730000-00-06, 753200-00-02, 753200-00-02, 762000-00-01, 762300-00-02, 762300-00-02, 773100-00-01</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>1750</v>
+        <v>1800</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[6]</t>
+          <t>[0.1]</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>324200-00-05</t>
+          <t>524504-50-01</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1755</v>
+        <v>1825</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>[0.2]</t>
+          <t>[4.6]</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>321100-03-09, 321100-03-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>1770</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>[0.1]</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>524504-50-01</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>1800</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>[4.7]</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>524504-50-01, 321100-00-15, 321100-00-15, 353100-00-02, 353103-00-01, 321100-01-09, 321100-01-09, 323200-50-01, 323200-50-01</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>1820</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>[0.2]</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>321100-03-09, 321100-03-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>1825</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>[4.0]</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>212700-00-01, 262400-00-02, 335000-02-04, 342200-00-01, 341100-50-01, 300000-50-01</t>
+          <t>212700-00-01, 262400-00-02, 335000-02-04, 342200-00-01, 341100-50-01, 300000-50-01, 300000-50-01, 300000-50-01</t>
         </is>
       </c>
     </row>

</xml_diff>